<commit_message>
Atualização relatorio de entrega
</commit_message>
<xml_diff>
--- a/Documentação/Parciais/Relatório de atividades ENTREGA_2.xlsx
+++ b/Documentação/Parciais/Relatório de atividades ENTREGA_2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Projeto_PHP\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\trabalhoFinal\Documentação\Parciais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5E6EBE-C310-46C6-873D-5F1D12AE7497}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B989DA89-FD82-4162-9565-BA3C65393964}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="570" windowWidth="19815" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Alunos</t>
   </si>
@@ -55,16 +55,28 @@
     <t>Leitura de configuração dinâmica do banco de dados</t>
   </si>
   <si>
-    <t>Seleção das tecnologias e padrões</t>
-  </si>
-  <si>
-    <t>Seleção da arquitetura</t>
-  </si>
-  <si>
     <t>Formalização do documento de entrega</t>
   </si>
   <si>
     <t>Modo de conexão dinâmica via reflexão</t>
+  </si>
+  <si>
+    <t>Pesquisa sobre a arquitetura</t>
+  </si>
+  <si>
+    <t>Pesquisa sobre as tecnologias e padrões</t>
+  </si>
+  <si>
+    <t>Justificativa do uso da arquitetura, tecnologias e padrões</t>
+  </si>
+  <si>
+    <t>Seleção da arquitetura, tecnologias e padrões</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Willian</t>
   </si>
 </sst>
 </file>
@@ -475,10 +487,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -515,7 +527,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -523,7 +535,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -534,10 +546,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
@@ -545,30 +557,47 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Update Documentação/Parciais/Relatório de atividades ENTREGA_2.xlsx
</commit_message>
<xml_diff>
--- a/Documentação/Parciais/Relatório de atividades ENTREGA_2.xlsx
+++ b/Documentação/Parciais/Relatório de atividades ENTREGA_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\trabalhoFinal\Documentação\Parciais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B989DA89-FD82-4162-9565-BA3C65393964}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCADF1C-3C4E-40D6-86AF-B26F61924EE4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="570" windowWidth="19815" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Alunos</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Willian</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -487,10 +490,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -599,6 +602,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>